<commit_message>
Started working on overall intro and discussion
</commit_message>
<xml_diff>
--- a/DEBkiss results/AIC stuff.xlsx
+++ b/DEBkiss results/AIC stuff.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\DEBkiss results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40797B63-207E-47EC-BB2B-D1AE3CD45193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACAF5C3-2132-4DDE-BEFC-B51C372BA777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Model</t>
   </si>
@@ -133,6 +134,18 @@
   </si>
   <si>
     <t>If yVA+muemb+mular is best</t>
+  </si>
+  <si>
+    <t>Weights (or Relative Likelihood)</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>Hatch Surv</t>
+  </si>
+  <si>
+    <t>Larv Surv</t>
   </si>
 </sst>
 </file>
@@ -501,29 +514,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15E1F97-C752-44B6-8BEC-CF43DE8C76A5}">
-  <dimension ref="B3:J23"/>
+  <dimension ref="B3:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -540,14 +554,17 @@
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -565,15 +582,19 @@
         <f>F5-$F$23</f>
         <v>16.080000000000041</v>
       </c>
-      <c r="I5">
+      <c r="H5">
+        <f>EXP(($F$23-F5)/2)</f>
+        <v>3.2230895011901227E-4</v>
+      </c>
+      <c r="J5">
         <v>600.70000000000005</v>
       </c>
-      <c r="J5">
-        <f>I5-$I$20</f>
+      <c r="K5">
+        <f>J5-$J$20</f>
         <v>15.950000000000045</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -591,15 +612,19 @@
         <f>F6-$F$23</f>
         <v>17.730000000000018</v>
       </c>
-      <c r="I6">
+      <c r="H6">
+        <f t="shared" ref="H6:H23" si="1">EXP(($F$23-F6)/2)</f>
+        <v>1.4124706032679263E-4</v>
+      </c>
+      <c r="J6">
         <v>602.35</v>
       </c>
-      <c r="J6">
-        <f t="shared" ref="J6:J23" si="1">I6-$I$20</f>
+      <c r="K6">
+        <f>J6-$J$20</f>
         <v>17.600000000000023</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -611,7 +636,7 @@
         <v>31.389999999999986</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -623,7 +648,7 @@
         <v>17.629999999999995</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -636,7 +661,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -654,15 +679,19 @@
         <f>F10-$F$23</f>
         <v>16</v>
       </c>
-      <c r="I10">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>3.3546262790251185E-4</v>
+      </c>
+      <c r="J10">
         <v>600.62</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="1"/>
+      <c r="K10">
+        <f>J10-$J$20</f>
         <v>15.870000000000005</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -680,15 +709,19 @@
         <f>F11-$F$23</f>
         <v>17.580000000000041</v>
       </c>
-      <c r="I11">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1.5224796768529346E-4</v>
+      </c>
+      <c r="J11">
         <v>602.20000000000005</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
+      <c r="K11">
+        <f>J11-$J$20</f>
         <v>17.450000000000045</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -700,7 +733,7 @@
         <v>14.699999999999932</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -718,15 +751,19 @@
         <f>F13-$F$23</f>
         <v>5.6499999999999773</v>
       </c>
-      <c r="I13">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>5.9308656829439407E-2</v>
+      </c>
+      <c r="J13">
         <v>590.27</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="1"/>
+      <c r="K13">
+        <f>J13-$J$20</f>
         <v>5.5199999999999818</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -744,15 +781,19 @@
         <f>F14-$F$23</f>
         <v>4.6399999999999864</v>
       </c>
-      <c r="I14">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>9.8273585604362196E-2</v>
+      </c>
+      <c r="J14">
         <v>589.26</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="1"/>
+      <c r="K14">
+        <f>J14-$J$20</f>
         <v>4.5099999999999909</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -764,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -782,15 +823,19 @@
         <f>F16-$F$23</f>
         <v>10.799999999999955</v>
       </c>
-      <c r="I16">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>4.5165809426127709E-3</v>
+      </c>
+      <c r="J16">
         <v>595.41999999999996</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="1"/>
+      <c r="K16">
+        <f>J16-$J$20</f>
         <v>10.669999999999959</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -808,15 +853,19 @@
         <f>F17-$F$23</f>
         <v>10.019999999999982</v>
       </c>
-      <c r="I17">
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>6.6709033062553333E-3</v>
+      </c>
+      <c r="J17">
         <v>594.64</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="1"/>
+      <c r="K17">
+        <f>J17-$J$20</f>
         <v>9.8899999999999864</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -828,7 +877,7 @@
         <v>11.980000000000018</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -846,15 +895,19 @@
         <f>F19-$F$23</f>
         <v>2.1000000000000227</v>
       </c>
-      <c r="I19">
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0.34993774911115139</v>
+      </c>
+      <c r="J19">
         <v>586.72</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="1"/>
+      <c r="K19">
+        <f>J19-$J$20</f>
         <v>1.9700000000000273</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -872,15 +925,19 @@
         <f>F20-$F$23</f>
         <v>0.12999999999999545</v>
       </c>
-      <c r="I20">
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0.93706746337740554</v>
+      </c>
+      <c r="J20">
         <v>584.75</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="1"/>
+      <c r="K20">
+        <f>J20-$J$20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -892,7 +949,7 @@
         <v>10.689999999999941</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -910,15 +967,19 @@
         <f>F22-$F$23</f>
         <v>2.2100000000000364</v>
       </c>
-      <c r="I22">
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0.33121088224197498</v>
+      </c>
+      <c r="J22">
         <v>586.83000000000004</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="1"/>
+      <c r="K22">
+        <f>J22-$J$20</f>
         <v>2.0800000000000409</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -936,11 +997,15 @@
         <f>F23-$F$23</f>
         <v>0</v>
       </c>
-      <c r="I23">
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J23">
         <v>584.62</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
+      <c r="K23">
+        <f>J23-$J$20</f>
         <v>-0.12999999999999545</v>
       </c>
     </row>
@@ -951,6 +1016,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F41CBC-AB57-430B-B420-397C80804C9F}">
+  <dimension ref="B6:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>7.7</v>
+      </c>
+      <c r="C7">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4.2</v>
+      </c>
+      <c r="C8">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>3.1</v>
+      </c>
+      <c r="C9">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>2.7</v>
+      </c>
+      <c r="C10">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C869D8-148A-4A2B-A6BA-E1069B0B1A52}">
   <dimension ref="B2:R22"/>
   <sheetViews>

</xml_diff>

<commit_message>
Lots of changes wrapping up edits to Ch4
</commit_message>
<xml_diff>
--- a/DEBkiss results/AIC stuff.xlsx
+++ b/DEBkiss results/AIC stuff.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\DEBkiss results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACAF5C3-2132-4DDE-BEFC-B51C372BA777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CA58DF-DC07-4B78-BF84-430F1793FB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -146,6 +147,45 @@
   </si>
   <si>
     <t>Larv Surv</t>
+  </si>
+  <si>
+    <t>AICc</t>
+  </si>
+  <si>
+    <t>Alt total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For AICc assume that N is each data point as entered in the matlab script, not the data points multiplied by their weights. </t>
+  </si>
+  <si>
+    <t>AICc = AIC+(2p(p+1)/(n-p-1))</t>
+  </si>
+  <si>
+    <t>p=1</t>
+  </si>
+  <si>
+    <t>n=141</t>
+  </si>
+  <si>
+    <t>c=0.02877</t>
+  </si>
+  <si>
+    <t>dry wt</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>50 mm</t>
+  </si>
+  <si>
+    <t>L^3</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>delM</t>
   </si>
 </sst>
 </file>
@@ -195,11 +235,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,30 +555,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15E1F97-C752-44B6-8BEC-CF43DE8C76A5}">
-  <dimension ref="B3:K23"/>
+  <dimension ref="B3:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -547,24 +588,27 @@
       <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -575,26 +619,30 @@
         <f>C5-$C$15</f>
         <v>32.600000000000023</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="4">
+        <f>C5+((2*2)/(141-1-1))</f>
+        <v>600.72877697841727</v>
+      </c>
+      <c r="G5">
         <v>600.70000000000005</v>
       </c>
-      <c r="G5">
-        <f>F5-$F$23</f>
+      <c r="H5">
+        <f>G5-$G$23</f>
         <v>16.080000000000041</v>
       </c>
-      <c r="H5">
-        <f>EXP(($F$23-F5)/2)</f>
+      <c r="I5">
+        <f>EXP(($G$23-G5)/2)</f>
         <v>3.2230895011901227E-4</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>600.70000000000005</v>
       </c>
-      <c r="K5">
-        <f>J5-$J$20</f>
+      <c r="M5">
+        <f>L5-$L$20</f>
         <v>15.950000000000045</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -605,26 +653,30 @@
         <f t="shared" ref="D6:D23" si="0">C6-$C$15</f>
         <v>34.25</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="4">
+        <f t="shared" ref="E6:E23" si="1">C6+((2*2)/(141-1-1))</f>
+        <v>602.37877697841725</v>
+      </c>
+      <c r="G6">
         <v>602.35</v>
       </c>
-      <c r="G6">
-        <f>F6-$F$23</f>
+      <c r="H6">
+        <f>G6-$G$23</f>
         <v>17.730000000000018</v>
       </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H23" si="1">EXP(($F$23-F6)/2)</f>
+      <c r="I6">
+        <f t="shared" ref="I6:I23" si="2">EXP(($G$23-G6)/2)</f>
         <v>1.4124706032679263E-4</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>602.35</v>
       </c>
-      <c r="K6">
-        <f>J6-$J$20</f>
+      <c r="M6">
+        <f>L6-$L$20</f>
         <v>17.600000000000023</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -635,8 +687,12 @@
         <f t="shared" si="0"/>
         <v>31.389999999999986</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E7" s="4">
+        <f t="shared" si="1"/>
+        <v>599.51877697841724</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -647,8 +703,12 @@
         <f t="shared" si="0"/>
         <v>17.629999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>585.75877697841725</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -659,9 +719,13 @@
         <f t="shared" si="0"/>
         <v>6.92999999999995</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
+        <f t="shared" si="1"/>
+        <v>575.0587769784172</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -672,26 +736,30 @@
         <f t="shared" si="0"/>
         <v>32.519999999999982</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="4">
+        <f t="shared" si="1"/>
+        <v>600.64877697841723</v>
+      </c>
+      <c r="G10">
         <v>600.62</v>
       </c>
-      <c r="G10">
-        <f>F10-$F$23</f>
+      <c r="H10">
+        <f>G10-$G$23</f>
         <v>16</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
+      <c r="I10">
+        <f t="shared" si="2"/>
         <v>3.3546262790251185E-4</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>600.62</v>
       </c>
-      <c r="K10">
-        <f>J10-$J$20</f>
+      <c r="M10">
+        <f>L10-$L$20</f>
         <v>15.870000000000005</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -702,26 +770,30 @@
         <f t="shared" si="0"/>
         <v>34.100000000000023</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="4">
+        <f t="shared" si="1"/>
+        <v>602.22877697841727</v>
+      </c>
+      <c r="G11">
         <v>602.20000000000005</v>
       </c>
-      <c r="G11">
-        <f>F11-$F$23</f>
+      <c r="H11">
+        <f>G11-$G$23</f>
         <v>17.580000000000041</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
+      <c r="I11">
+        <f t="shared" si="2"/>
         <v>1.5224796768529346E-4</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>602.20000000000005</v>
       </c>
-      <c r="K11">
-        <f>J11-$J$20</f>
+      <c r="M11">
+        <f>L11-$L$20</f>
         <v>17.450000000000045</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -732,8 +804,12 @@
         <f t="shared" si="0"/>
         <v>14.699999999999932</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
+        <v>582.82877697841718</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -744,26 +820,30 @@
         <f t="shared" si="0"/>
         <v>22.169999999999959</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="4">
+        <f t="shared" si="1"/>
+        <v>590.29877697841721</v>
+      </c>
+      <c r="G13">
         <v>590.27</v>
       </c>
-      <c r="G13">
-        <f>F13-$F$23</f>
+      <c r="H13">
+        <f>G13-$G$23</f>
         <v>5.6499999999999773</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
+      <c r="I13">
+        <f t="shared" si="2"/>
         <v>5.9308656829439407E-2</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>590.27</v>
       </c>
-      <c r="K13">
-        <f>J13-$J$20</f>
+      <c r="M13">
+        <f>L13-$L$20</f>
         <v>5.5199999999999818</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -774,26 +854,30 @@
         <f t="shared" si="0"/>
         <v>21.159999999999968</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="4">
+        <f t="shared" si="1"/>
+        <v>589.28877697841722</v>
+      </c>
+      <c r="G14">
         <v>589.26</v>
       </c>
-      <c r="G14">
-        <f>F14-$F$23</f>
+      <c r="H14">
+        <f>G14-$G$23</f>
         <v>4.6399999999999864</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
+      <c r="I14">
+        <f t="shared" si="2"/>
         <v>9.8273585604362196E-2</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>589.26</v>
       </c>
-      <c r="K14">
-        <f>J14-$J$20</f>
+      <c r="M14">
+        <f>L14-$L$20</f>
         <v>4.5099999999999909</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -804,8 +888,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>568.12877697841725</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -816,26 +904,30 @@
         <f t="shared" si="0"/>
         <v>27.319999999999936</v>
       </c>
-      <c r="F16">
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>595.44877697841719</v>
+      </c>
+      <c r="G16">
         <v>595.41999999999996</v>
       </c>
-      <c r="G16">
-        <f>F16-$F$23</f>
+      <c r="H16">
+        <f>G16-$G$23</f>
         <v>10.799999999999955</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
+      <c r="I16">
+        <f t="shared" si="2"/>
         <v>4.5165809426127709E-3</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>595.41999999999996</v>
       </c>
-      <c r="K16">
-        <f>J16-$J$20</f>
+      <c r="M16">
+        <f>L16-$L$20</f>
         <v>10.669999999999959</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -846,26 +938,30 @@
         <f t="shared" si="0"/>
         <v>26.539999999999964</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>594.66877697841721</v>
+      </c>
+      <c r="G17">
         <v>594.64</v>
       </c>
-      <c r="G17">
-        <f>F17-$F$23</f>
+      <c r="H17">
+        <f>G17-$G$23</f>
         <v>10.019999999999982</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
+      <c r="I17">
+        <f t="shared" si="2"/>
         <v>6.6709033062553333E-3</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>594.64</v>
       </c>
-      <c r="K17">
-        <f>J17-$J$20</f>
+      <c r="M17">
+        <f>L17-$L$20</f>
         <v>9.8899999999999864</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -876,8 +972,12 @@
         <f t="shared" si="0"/>
         <v>11.980000000000018</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>580.10877697841727</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -888,26 +988,30 @@
         <f t="shared" si="0"/>
         <v>18.620000000000005</v>
       </c>
-      <c r="F19">
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>586.74877697841725</v>
+      </c>
+      <c r="G19">
         <v>586.72</v>
       </c>
-      <c r="G19" s="2">
-        <f>F19-$F$23</f>
+      <c r="H19" s="2">
+        <f>G19-$G$23</f>
         <v>2.1000000000000227</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
+      <c r="I19">
+        <f t="shared" si="2"/>
         <v>0.34993774911115139</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>586.72</v>
       </c>
-      <c r="K19">
-        <f>J19-$J$20</f>
+      <c r="M19">
+        <f>L19-$L$20</f>
         <v>1.9700000000000273</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -918,26 +1022,30 @@
         <f t="shared" si="0"/>
         <v>16.649999999999977</v>
       </c>
-      <c r="F20">
+      <c r="E20" s="4">
+        <f t="shared" si="1"/>
+        <v>584.77877697841723</v>
+      </c>
+      <c r="G20">
         <v>584.75</v>
       </c>
-      <c r="G20" s="2">
-        <f>F20-$F$23</f>
+      <c r="H20" s="2">
+        <f>G20-$G$23</f>
         <v>0.12999999999999545</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
+      <c r="I20">
+        <f t="shared" si="2"/>
         <v>0.93706746337740554</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>584.75</v>
       </c>
-      <c r="K20">
-        <f>J20-$J$20</f>
+      <c r="M20">
+        <f>L20-$L$20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -948,8 +1056,12 @@
         <f t="shared" si="0"/>
         <v>10.689999999999941</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E21" s="4">
+        <f t="shared" si="1"/>
+        <v>578.81877697841719</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -960,26 +1072,30 @@
         <f t="shared" si="0"/>
         <v>18.730000000000018</v>
       </c>
-      <c r="F22">
+      <c r="E22" s="4">
+        <f t="shared" si="1"/>
+        <v>586.85877697841727</v>
+      </c>
+      <c r="G22">
         <v>586.83000000000004</v>
       </c>
-      <c r="G22">
-        <f>F22-$F$23</f>
+      <c r="H22">
+        <f>G22-$G$23</f>
         <v>2.2100000000000364</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
+      <c r="I22">
+        <f t="shared" si="2"/>
         <v>0.33121088224197498</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>586.83000000000004</v>
       </c>
-      <c r="K22">
-        <f>J22-$J$20</f>
+      <c r="M22">
+        <f>L22-$L$20</f>
         <v>2.0800000000000409</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -990,23 +1106,52 @@
         <f t="shared" si="0"/>
         <v>16.519999999999982</v>
       </c>
-      <c r="F23">
+      <c r="E23" s="4">
+        <f t="shared" si="1"/>
+        <v>584.64877697841723</v>
+      </c>
+      <c r="G23">
         <v>584.62</v>
       </c>
-      <c r="G23">
-        <f>F23-$F$23</f>
+      <c r="H23">
+        <f>G23-$G$23</f>
         <v>0</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
+      <c r="I23">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>584.62</v>
       </c>
-      <c r="K23">
-        <f>J23-$J$20</f>
+      <c r="M23">
+        <f>L23-$L$20</f>
         <v>-0.12999999999999545</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1019,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F41CBC-AB57-430B-B420-397C80804C9F}">
   <dimension ref="B6:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1090,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C869D8-148A-4A2B-A6BA-E1069B0B1A52}">
-  <dimension ref="B2:R22"/>
+  <dimension ref="B2:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1349,6 +1494,12 @@
       <c r="J14">
         <v>50</v>
       </c>
+      <c r="M14" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14">
+        <v>8</v>
+      </c>
       <c r="Q14">
         <v>47</v>
       </c>
@@ -1385,7 +1536,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I17">
         <v>56</v>
       </c>
@@ -1393,15 +1544,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I18">
         <v>64</v>
       </c>
       <c r="J18">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="Q18" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I19">
         <v>86</v>
       </c>
@@ -1409,7 +1566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I20">
         <v>103</v>
       </c>
@@ -1417,7 +1574,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I21">
         <v>110</v>
       </c>
@@ -1425,7 +1582,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I22" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1591,75 @@
         <v>1293</v>
       </c>
     </row>
+    <row r="24" spans="9:18" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C64110-9B40-4C3C-A936-92ACE2439C25}">
+  <dimension ref="S15:T19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="15" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S16" t="s">
+        <v>43</v>
+      </c>
+      <c r="T16">
+        <f>EXP((2.997*LN(50))-6.7)</f>
+        <v>152.06878437488612</v>
+      </c>
+    </row>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S17" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17">
+        <f>152.0688/0.4</f>
+        <v>380.17200000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>47</v>
+      </c>
+      <c r="T18">
+        <f>T17^(1/3)</f>
+        <v>7.2442491057130214</v>
+      </c>
+    </row>
+    <row r="19" spans="19:20" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19">
+        <f>T18/50</f>
+        <v>0.14488498211426043</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ch4 edits from Roger
</commit_message>
<xml_diff>
--- a/DEBkiss results/AIC stuff.xlsx
+++ b/DEBkiss results/AIC stuff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\DEBkiss results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CA58DF-DC07-4B78-BF84-430F1793FB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E392E3-78F7-40B6-92B8-9B3BA49DED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>Model</t>
   </si>
@@ -137,9 +138,6 @@
     <t>If yVA+muemb+mular is best</t>
   </si>
   <si>
-    <t>Weights (or Relative Likelihood)</t>
-  </si>
-  <si>
     <t>DO</t>
   </si>
   <si>
@@ -186,6 +184,15 @@
   </si>
   <si>
     <t>delM</t>
+  </si>
+  <si>
+    <t>Relative likelihood</t>
+  </si>
+  <si>
+    <t>Akaike Weights</t>
+  </si>
+  <si>
+    <t>Akaike weight</t>
   </si>
 </sst>
 </file>
@@ -555,19 +562,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15E1F97-C752-44B6-8BEC-CF43DE8C76A5}">
-  <dimension ref="B3:M35"/>
+  <dimension ref="B3:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>29</v>
       </c>
@@ -578,7 +586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -589,7 +597,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
@@ -599,7 +607,10 @@
         <v>28</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>2</v>
@@ -608,7 +619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -631,8 +642,12 @@
         <v>16.080000000000041</v>
       </c>
       <c r="I5">
-        <f>EXP(($G$23-G5)/2)</f>
+        <f>EXP(-H5/2)</f>
         <v>3.2230895011901227E-4</v>
+      </c>
+      <c r="J5">
+        <f>I5/$I$24</f>
+        <v>1.1560840146073931E-4</v>
       </c>
       <c r="L5">
         <v>600.70000000000005</v>
@@ -642,7 +657,7 @@
         <v>15.950000000000045</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -665,8 +680,12 @@
         <v>17.730000000000018</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I23" si="2">EXP(($G$23-G6)/2)</f>
+        <f t="shared" ref="I6:I23" si="2">EXP(-H6/2)</f>
         <v>1.4124706032679263E-4</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J23" si="3">I6/$I$24</f>
+        <v>5.066364694303249E-5</v>
       </c>
       <c r="L6">
         <v>602.35</v>
@@ -676,7 +695,7 @@
         <v>17.600000000000023</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -691,8 +710,18 @@
         <f t="shared" si="1"/>
         <v>599.51877697841724</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7">
+        <v>0.35868815128481857</v>
+      </c>
+      <c r="T7">
+        <f>S7/S8</f>
+        <v>1.0671590243841904</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -707,8 +736,14 @@
         <f t="shared" si="1"/>
         <v>585.75877697841725</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8">
+        <v>0.336114996067996</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -725,7 +760,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -751,6 +786,10 @@
         <f t="shared" si="2"/>
         <v>3.3546262790251185E-4</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>1.2032646982749897E-4</v>
+      </c>
       <c r="L10">
         <v>600.62</v>
       </c>
@@ -759,7 +798,7 @@
         <v>15.870000000000005</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -785,6 +824,10 @@
         <f t="shared" si="2"/>
         <v>1.5224796768529346E-4</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>5.4609542065908705E-5</v>
+      </c>
       <c r="L11">
         <v>602.20000000000005</v>
       </c>
@@ -793,7 +836,7 @@
         <v>17.450000000000045</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -808,8 +851,18 @@
         <f t="shared" si="1"/>
         <v>582.82877697841718</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12">
+        <v>0.336114996067996</v>
+      </c>
+      <c r="T12">
+        <f>S12/S13</f>
+        <v>2.6778118844210859</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -835,6 +888,10 @@
         <f t="shared" si="2"/>
         <v>5.9308656829439407E-2</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>2.1273312473337351E-2</v>
+      </c>
       <c r="L13">
         <v>590.27</v>
       </c>
@@ -842,8 +899,14 @@
         <f>L13-$L$20</f>
         <v>5.5199999999999818</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13">
+        <v>0.12551852429344956</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -869,6 +932,10 @@
         <f t="shared" si="2"/>
         <v>9.8273585604362196E-2</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>3.5249570740559032E-2</v>
+      </c>
       <c r="L14">
         <v>589.26</v>
       </c>
@@ -877,7 +944,7 @@
         <v>4.5099999999999909</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -893,7 +960,7 @@
         <v>568.12877697841725</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -919,6 +986,10 @@
         <f t="shared" si="2"/>
         <v>4.5165809426127709E-3</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>1.620044068434018E-3</v>
+      </c>
       <c r="L16">
         <v>595.41999999999996</v>
       </c>
@@ -927,7 +998,7 @@
         <v>10.669999999999959</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -953,6 +1024,10 @@
         <f t="shared" si="2"/>
         <v>6.6709033062553333E-3</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>2.3927739743205092E-3</v>
+      </c>
       <c r="L17">
         <v>594.64</v>
       </c>
@@ -961,7 +1036,7 @@
         <v>9.8899999999999864</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -976,8 +1051,18 @@
         <f t="shared" si="1"/>
         <v>580.10877697841727</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S18">
+        <v>0.35868815128481857</v>
+      </c>
+      <c r="T18">
+        <f>S18/S19</f>
+        <v>221.40641620418205</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -1003,6 +1088,10 @@
         <f t="shared" si="2"/>
         <v>0.34993774911115139</v>
       </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>0.12551852429344956</v>
+      </c>
       <c r="L19">
         <v>586.72</v>
       </c>
@@ -1010,8 +1099,14 @@
         <f>L19-$L$20</f>
         <v>1.9700000000000273</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R19" t="s">
+        <v>17</v>
+      </c>
+      <c r="S19">
+        <v>1.620044068434018E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -1037,6 +1132,10 @@
         <f t="shared" si="2"/>
         <v>0.93706746337740554</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>0.336114996067996</v>
+      </c>
       <c r="L20">
         <v>584.75</v>
       </c>
@@ -1045,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -1061,7 +1160,7 @@
         <v>578.81877697841719</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>26</v>
       </c>
@@ -1087,6 +1186,10 @@
         <f t="shared" si="2"/>
         <v>0.33121088224197498</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>0.11880141903678774</v>
+      </c>
       <c r="L22">
         <v>586.83000000000004</v>
       </c>
@@ -1095,7 +1198,7 @@
         <v>2.0800000000000409</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -1121,6 +1224,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>0.35868815128481857</v>
+      </c>
       <c r="L23">
         <v>584.62</v>
       </c>
@@ -1128,30 +1235,56 @@
         <f>L23-$L$20</f>
         <v>-0.12999999999999545</v>
       </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="R23" t="s">
+        <v>27</v>
+      </c>
+      <c r="S23">
+        <v>0.35868815128481857</v>
+      </c>
+      <c r="T23">
+        <f>S23/S24</f>
+        <v>10.175674306073267</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <f>SUM(I5:I23)</f>
+        <v>2.7879370880192353</v>
+      </c>
+      <c r="J24">
+        <f>SUM(J5:J23)</f>
+        <v>1</v>
+      </c>
+      <c r="R24" t="s">
+        <v>18</v>
+      </c>
+      <c r="S24">
+        <v>3.5249570740559032E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1175,13 +1308,13 @@
   <sheetData>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
@@ -1495,7 +1628,7 @@
         <v>50</v>
       </c>
       <c r="M14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N14">
         <v>8</v>
@@ -1552,7 +1685,7 @@
         <v>36</v>
       </c>
       <c r="Q18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R18">
         <v>12</v>
@@ -1593,7 +1726,7 @@
     </row>
     <row r="24" spans="9:18" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J24">
         <v>121</v>
@@ -1616,15 +1749,15 @@
   <sheetData>
     <row r="15" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S15" t="s">
+        <v>43</v>
+      </c>
+      <c r="T15" t="s">
         <v>44</v>
-      </c>
-      <c r="T15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T16">
         <f>EXP((2.997*LN(50))-6.7)</f>
@@ -1633,7 +1766,7 @@
     </row>
     <row r="17" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T17">
         <f>152.0688/0.4</f>
@@ -1642,7 +1775,7 @@
     </row>
     <row r="18" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T18">
         <f>T17^(1/3)</f>
@@ -1651,7 +1784,7 @@
     </row>
     <row r="19" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T19">
         <f>T18/50</f>
@@ -1662,4 +1795,368 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DCB310-4BB0-4F95-8F30-69632E6C18DD}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>602.35</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="0">B3-$B$10</f>
+        <v>34.25</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D15" si="1">B3+((2*2)/(141-1-1))</f>
+        <v>602.37877697841725</v>
+      </c>
+      <c r="F3">
+        <v>602.35</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G14" si="2">F3-$F$15</f>
+        <v>17.730000000000018</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H15" si="3">EXP(-G3/2)</f>
+        <v>1.4124706032679263E-4</v>
+      </c>
+      <c r="I3">
+        <f>H3/$H$16</f>
+        <v>6.9160595205000923E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>599.49</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>31.389999999999986</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>599.51877697841724</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>585.73</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>17.629999999999995</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>585.75877697841725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>575.03</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.92999999999995</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>575.0587769784172</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>602.20000000000005</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>34.100000000000023</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>602.22877697841727</v>
+      </c>
+      <c r="F7">
+        <v>602.20000000000005</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>17.580000000000041</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>1.5224796768529346E-4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I4:I15" si="4">H7/$H$16</f>
+        <v>7.454710943721728E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>582.79999999999995</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>14.699999999999932</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>582.82877697841718</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>589.26</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>21.159999999999968</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>589.28877697841722</v>
+      </c>
+      <c r="F9">
+        <v>589.26</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>4.6399999999999864</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>9.8273585604362196E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>4.8118946034008653E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>568.1</v>
+      </c>
+      <c r="C10">
+        <f>B10-$B$10</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>568.12877697841725</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>594.64</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C15" si="5">B11-$B$10</f>
+        <v>26.539999999999964</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>594.66877697841721</v>
+      </c>
+      <c r="F11">
+        <v>594.64</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>10.019999999999982</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>6.6709033062553333E-3</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>3.2663592583676094E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>580.08000000000004</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="5"/>
+        <v>11.980000000000018</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>580.10877697841727</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>584.75</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="5"/>
+        <v>16.649999999999977</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>584.77877697841723</v>
+      </c>
+      <c r="F13">
+        <v>584.75</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0.12999999999999545</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>0.93706746337740554</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="4"/>
+        <v>0.4588282642093936</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>578.79</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="5"/>
+        <v>10.689999999999941</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>578.81877697841719</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>584.62</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="5"/>
+        <v>16.519999999999982</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>584.64877697841723</v>
+      </c>
+      <c r="F15">
+        <v>584.62</v>
+      </c>
+      <c r="G15">
+        <f>F15-$F$15</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="4"/>
+        <v>0.48964272279358795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <f>SUM(H3:H15)</f>
+        <v>2.0423054473160351</v>
+      </c>
+      <c r="I16">
+        <f>SUM(I3:I15)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
a lot of change relating to DEB paper
</commit_message>
<xml_diff>
--- a/DEBkiss results/AIC stuff.xlsx
+++ b/DEBkiss results/AIC stuff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\DEBkiss results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E392E3-78F7-40B6-92B8-9B3BA49DED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E554C5-BC8D-4E1F-AC38-971EAF0A825E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="6" xr2:uid="{797BED97-2A8B-4207-9B37-E76789808921}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
   <si>
     <t>Model</t>
   </si>
@@ -193,6 +195,63 @@
   </si>
   <si>
     <t>Akaike weight</t>
+  </si>
+  <si>
+    <t>JaAm + uemb</t>
+  </si>
+  <si>
+    <t>yVA + uemb</t>
+  </si>
+  <si>
+    <t>JvM + uemb</t>
+  </si>
+  <si>
+    <t>JaAm + ular</t>
+  </si>
+  <si>
+    <t>yVA + ular</t>
+  </si>
+  <si>
+    <t>JvM + ular</t>
+  </si>
+  <si>
+    <t>JaAm + uemb + ular</t>
+  </si>
+  <si>
+    <t>yVA + uemb + ular</t>
+  </si>
+  <si>
+    <t>JvM + uemb + ular</t>
+  </si>
+  <si>
+    <t>uemb + ular</t>
+  </si>
+  <si>
+    <t>Updated AIC values after using inhibition as correction factor</t>
+  </si>
+  <si>
+    <t>All models</t>
+  </si>
+  <si>
+    <t>Original value</t>
+  </si>
+  <si>
+    <t>mu_emb</t>
+  </si>
+  <si>
+    <t>mu_lar</t>
+  </si>
+  <si>
+    <t>y_VA</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>UL</t>
   </si>
 </sst>
 </file>
@@ -242,11 +301,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -564,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15E1F97-C752-44B6-8BEC-CF43DE8C76A5}">
   <dimension ref="B3:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +688,7 @@
         <f>C5-$C$15</f>
         <v>32.600000000000023</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f>C5+((2*2)/(141-1-1))</f>
         <v>600.72877697841727</v>
       </c>
@@ -668,7 +726,7 @@
         <f t="shared" ref="D6:D23" si="0">C6-$C$15</f>
         <v>34.25</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f t="shared" ref="E6:E23" si="1">C6+((2*2)/(141-1-1))</f>
         <v>602.37877697841725</v>
       </c>
@@ -706,7 +764,7 @@
         <f t="shared" si="0"/>
         <v>31.389999999999986</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f t="shared" si="1"/>
         <v>599.51877697841724</v>
       </c>
@@ -732,7 +790,7 @@
         <f t="shared" si="0"/>
         <v>17.629999999999995</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <f t="shared" si="1"/>
         <v>585.75877697841725</v>
       </c>
@@ -750,15 +808,14 @@
       <c r="C9">
         <v>575.03</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>6.92999999999995</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f t="shared" si="1"/>
         <v>575.0587769784172</v>
       </c>
-      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -771,7 +828,7 @@
         <f t="shared" si="0"/>
         <v>32.519999999999982</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f t="shared" si="1"/>
         <v>600.64877697841723</v>
       </c>
@@ -809,7 +866,7 @@
         <f t="shared" si="0"/>
         <v>34.100000000000023</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f t="shared" si="1"/>
         <v>602.22877697841727</v>
       </c>
@@ -847,7 +904,7 @@
         <f t="shared" si="0"/>
         <v>14.699999999999932</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <f t="shared" si="1"/>
         <v>582.82877697841718</v>
       </c>
@@ -873,7 +930,7 @@
         <f t="shared" si="0"/>
         <v>22.169999999999959</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <f t="shared" si="1"/>
         <v>590.29877697841721</v>
       </c>
@@ -917,7 +974,7 @@
         <f t="shared" si="0"/>
         <v>21.159999999999968</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" si="1"/>
         <v>589.28877697841722</v>
       </c>
@@ -955,7 +1012,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f t="shared" si="1"/>
         <v>568.12877697841725</v>
       </c>
@@ -971,7 +1028,7 @@
         <f t="shared" si="0"/>
         <v>27.319999999999936</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" si="1"/>
         <v>595.44877697841719</v>
       </c>
@@ -1009,7 +1066,7 @@
         <f t="shared" si="0"/>
         <v>26.539999999999964</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
         <v>594.66877697841721</v>
       </c>
@@ -1047,7 +1104,7 @@
         <f t="shared" si="0"/>
         <v>11.980000000000018</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <f t="shared" si="1"/>
         <v>580.10877697841727</v>
       </c>
@@ -1073,7 +1130,7 @@
         <f t="shared" si="0"/>
         <v>18.620000000000005</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <f t="shared" si="1"/>
         <v>586.74877697841725</v>
       </c>
@@ -1117,7 +1174,7 @@
         <f t="shared" si="0"/>
         <v>16.649999999999977</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f t="shared" si="1"/>
         <v>584.77877697841723</v>
       </c>
@@ -1155,7 +1212,7 @@
         <f t="shared" si="0"/>
         <v>10.689999999999941</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <f t="shared" si="1"/>
         <v>578.81877697841719</v>
       </c>
@@ -1171,7 +1228,7 @@
         <f t="shared" si="0"/>
         <v>18.730000000000018</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <f t="shared" si="1"/>
         <v>586.85877697841727</v>
       </c>
@@ -1209,7 +1266,7 @@
         <f t="shared" si="0"/>
         <v>16.519999999999982</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <f t="shared" si="1"/>
         <v>584.64877697841723</v>
       </c>
@@ -1858,7 +1915,7 @@
         <f t="shared" ref="C3:C9" si="0">B3-$B$10</f>
         <v>34.25</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D15" si="1">B3+((2*2)/(141-1-1))</f>
         <v>602.37877697841725</v>
       </c>
@@ -1866,7 +1923,7 @@
         <v>602.35</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G14" si="2">F3-$F$15</f>
+        <f t="shared" ref="G3:G13" si="2">F3-$F$15</f>
         <v>17.730000000000018</v>
       </c>
       <c r="H3">
@@ -1889,7 +1946,7 @@
         <f t="shared" si="0"/>
         <v>31.389999999999986</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f t="shared" si="1"/>
         <v>599.51877697841724</v>
       </c>
@@ -1905,7 +1962,7 @@
         <f t="shared" si="0"/>
         <v>17.629999999999995</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" si="1"/>
         <v>585.75877697841725</v>
       </c>
@@ -1921,11 +1978,10 @@
         <f t="shared" si="0"/>
         <v>6.92999999999995</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
         <v>575.0587769784172</v>
       </c>
-      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1938,7 +1994,7 @@
         <f t="shared" si="0"/>
         <v>34.100000000000023</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" si="1"/>
         <v>602.22877697841727</v>
       </c>
@@ -1954,7 +2010,7 @@
         <v>1.5224796768529346E-4</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I4:I15" si="4">H7/$H$16</f>
+        <f t="shared" ref="I7:I15" si="4">H7/$H$16</f>
         <v>7.454710943721728E-5</v>
       </c>
     </row>
@@ -1969,7 +2025,7 @@
         <f t="shared" si="0"/>
         <v>14.699999999999932</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="1"/>
         <v>582.82877697841718</v>
       </c>
@@ -1985,7 +2041,7 @@
         <f t="shared" si="0"/>
         <v>21.159999999999968</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="1"/>
         <v>589.28877697841722</v>
       </c>
@@ -2016,7 +2072,7 @@
         <f>B10-$B$10</f>
         <v>0</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="1"/>
         <v>568.12877697841725</v>
       </c>
@@ -2032,7 +2088,7 @@
         <f t="shared" ref="C11:C15" si="5">B11-$B$10</f>
         <v>26.539999999999964</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" si="1"/>
         <v>594.66877697841721</v>
       </c>
@@ -2063,7 +2119,7 @@
         <f t="shared" si="5"/>
         <v>11.980000000000018</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <f t="shared" si="1"/>
         <v>580.10877697841727</v>
       </c>
@@ -2079,7 +2135,7 @@
         <f t="shared" si="5"/>
         <v>16.649999999999977</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <f t="shared" si="1"/>
         <v>584.77877697841723</v>
       </c>
@@ -2110,7 +2166,7 @@
         <f t="shared" si="5"/>
         <v>10.689999999999941</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" si="1"/>
         <v>578.81877697841719</v>
       </c>
@@ -2126,7 +2182,7 @@
         <f t="shared" si="5"/>
         <v>16.519999999999982</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" si="1"/>
         <v>584.64877697841723</v>
       </c>
@@ -2159,4 +2215,1148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66780FD8-7105-409E-A08A-697104985B98}">
+  <dimension ref="B2:P24"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>856.03</v>
+      </c>
+      <c r="D5">
+        <f>C5-$C$9</f>
+        <v>94.889999999999986</v>
+      </c>
+      <c r="E5" s="3">
+        <f>C5+((2*2)/(141-1-1))</f>
+        <v>856.0587769784172</v>
+      </c>
+      <c r="H5">
+        <v>856.03</v>
+      </c>
+      <c r="I5">
+        <f>H5-$H$9</f>
+        <v>94.889999999999986</v>
+      </c>
+      <c r="J5">
+        <f>EXP(-I5/2)</f>
+        <v>2.4825517257544032E-21</v>
+      </c>
+      <c r="K5">
+        <f>J5/$J$24</f>
+        <v>2.4266125651005946E-21</v>
+      </c>
+      <c r="M5">
+        <v>856.03</v>
+      </c>
+      <c r="N5">
+        <f>M5-$M$20</f>
+        <v>62.029999999999973</v>
+      </c>
+      <c r="O5">
+        <f>EXP(-N5/2)</f>
+        <v>3.3912253013640474E-14</v>
+      </c>
+      <c r="P5">
+        <f>O5/$O$24</f>
+        <v>2.4563230741904939E-14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>848.62</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D23" si="0">C6-$C$9</f>
+        <v>87.480000000000018</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" ref="E6:E23" si="1">C6+((2*2)/(141-1-1))</f>
+        <v>848.64877697841723</v>
+      </c>
+      <c r="H6">
+        <v>848.62</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I23" si="2">H6-$H$9</f>
+        <v>87.480000000000018</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J23" si="3">EXP(-I6/2)</f>
+        <v>1.0091584511851394E-19</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ref="K6:K24" si="4">J6/$J$24</f>
+        <v>9.8641915591070165E-20</v>
+      </c>
+      <c r="M6">
+        <v>848.62</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N23" si="5">M6-$M$20</f>
+        <v>54.620000000000005</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O23" si="6">EXP(-N6/2)</f>
+        <v>1.3785346896264282E-12</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P24" si="7">O6/$O$24</f>
+        <v>9.9849649191383113E-13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>849.19</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>88.050000000000068</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>849.21877697841728</v>
+      </c>
+      <c r="H7">
+        <v>849.19</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>88.050000000000068</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>7.5890154015807678E-20</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="4"/>
+        <v>7.4180126597852265E-20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>792.38</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>31.240000000000009</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>792.40877697841722</v>
+      </c>
+      <c r="H8">
+        <v>792.38</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>31.240000000000009</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>1.645584517612598E-7</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>1.6085046792570938E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>761.14</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="1"/>
+        <v>761.16877697841721</v>
+      </c>
+      <c r="H9">
+        <v>761.14</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="4"/>
+        <v>0.97746707145172984</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>854.97</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>93.830000000000041</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="1"/>
+        <v>854.99877697841725</v>
+      </c>
+      <c r="H10">
+        <v>854.97</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>93.830000000000041</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>4.2176873347007804E-21</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>4.1226504873490234E-21</v>
+      </c>
+      <c r="M10">
+        <v>854.97</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="5"/>
+        <v>60.970000000000027</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="6"/>
+        <v>5.7614622302919048E-14</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="7"/>
+        <v>4.1731266311473576E-14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>850.61</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>89.470000000000027</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="1"/>
+        <v>850.63877697841724</v>
+      </c>
+      <c r="H11">
+        <v>850.61</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>89.470000000000027</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>3.7310953866291563E-20</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="4"/>
+        <v>3.6470228808754611E-20</v>
+      </c>
+      <c r="M11">
+        <v>850.61</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="5"/>
+        <v>56.610000000000014</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="6"/>
+        <v>5.0967659387215591E-13</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="7"/>
+        <v>3.6916756235553908E-13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>823.21</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>62.07000000000005</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>823.23877697841726</v>
+      </c>
+      <c r="H12">
+        <v>823.21</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>62.07000000000005</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>3.3240745412812121E-14</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>3.2491734071533988E-14</v>
+      </c>
+      <c r="M12">
+        <v>823.21</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="5"/>
+        <v>29.210000000000036</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="6"/>
+        <v>4.5407656851892456E-7</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="7"/>
+        <v>3.288955034198542E-7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>808.09</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>46.950000000000045</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="1"/>
+        <v>808.11877697841726</v>
+      </c>
+      <c r="H13">
+        <v>808.09</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>46.950000000000045</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>6.3817095941980243E-11</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>6.2379109878961503E-11</v>
+      </c>
+      <c r="M13">
+        <v>808.09</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="5"/>
+        <v>14.090000000000032</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="6"/>
+        <v>8.7175686279912122E-4</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="7"/>
+        <v>6.314285566093469E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <v>796.52</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>35.379999999999995</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>796.54877697841721</v>
+      </c>
+      <c r="H14">
+        <v>796.52</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>35.379999999999995</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>2.0764936871665619E-8</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>2.0297042032827036E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15">
+        <v>838.14</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>838.16877697841721</v>
+      </c>
+      <c r="H15">
+        <v>838.14</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>1.9039802832864523E-17</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>1.8610780316058435E-17</v>
+      </c>
+      <c r="M15">
+        <v>838.14</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="5"/>
+        <v>44.139999999999986</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="6"/>
+        <v>2.6008828106158351E-10</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="7"/>
+        <v>1.8838643538108247E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>821.27</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>60.129999999999995</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>821.29877697841721</v>
+      </c>
+      <c r="H16">
+        <v>821.27</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>60.129999999999995</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>8.7687240186532088E-14</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>8.5711389868813956E-14</v>
+      </c>
+      <c r="M16">
+        <v>821.27</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="5"/>
+        <v>27.269999999999982</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="6"/>
+        <v>1.1978287680470759E-6</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="7"/>
+        <v>8.6760807095292288E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>768.86</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>7.7200000000000273</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="1"/>
+        <v>768.88877697841724</v>
+      </c>
+      <c r="H17">
+        <v>768.86</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>7.7200000000000273</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>2.1067999523041142E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>2.0593275795133467E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>773.88</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>12.740000000000009</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="1"/>
+        <v>773.90877697841722</v>
+      </c>
+      <c r="H18">
+        <v>773.88</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>12.740000000000009</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>1.7121592255655153E-3</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>1.673579264072586E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <v>810.18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>49.039999999999964</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="1"/>
+        <v>810.20877697841718</v>
+      </c>
+      <c r="H19">
+        <v>810.18</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>49.039999999999964</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>2.24439505792606E-11</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>2.1938222644517215E-11</v>
+      </c>
+      <c r="M19">
+        <v>810.18</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="5"/>
+        <v>16.17999999999995</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>3.0658975713315127E-4</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
+        <v>2.2206825788121697E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <v>794</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>32.860000000000014</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>794.02877697841723</v>
+      </c>
+      <c r="H20">
+        <v>794</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>32.860000000000014</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>7.3205154631155009E-8</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>7.155562811248613E-8</v>
+      </c>
+      <c r="M20">
+        <v>794</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="7"/>
+        <v>0.72431727647304667</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <v>777.56</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>16.419999999999959</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>777.58877697841717</v>
+      </c>
+      <c r="H21">
+        <v>777.56</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>16.419999999999959</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>2.7192072128954056E-4</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="4"/>
+        <v>2.6579355110592924E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>809.93</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>48.789999999999964</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="1"/>
+        <v>809.95877697841718</v>
+      </c>
+      <c r="H22">
+        <v>809.93</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>48.789999999999964</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>2.5432327879597447E-11</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>2.4859263052670299E-11</v>
+      </c>
+      <c r="M22">
+        <v>809.93</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="5"/>
+        <v>15.92999999999995</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="6"/>
+        <v>3.4741170902156439E-4</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="7"/>
+        <v>2.5163630289334611E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>795.94</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>34.800000000000068</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="1"/>
+        <v>795.96877697841728</v>
+      </c>
+      <c r="H23">
+        <v>795.94</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>34.800000000000068</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>2.7750832422406577E-8</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>2.7125524898277469E-8</v>
+      </c>
+      <c r="M23">
+        <v>795.94</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="5"/>
+        <v>1.9400000000000546</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="6"/>
+        <v>0.37908303810338845</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="7"/>
+        <v>0.27457639371617448</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <f>SUM(J5:J23)</f>
+        <v>1.0230523658610866</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <f>SUM(O5:O23)</f>
+        <v>1.380610448599747</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA32AEA-C6BC-4EE0-B7D8-2524E1A65524}">
+  <dimension ref="A6:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>7.7</v>
+      </c>
+      <c r="E6">
+        <v>4.2</v>
+      </c>
+      <c r="F6">
+        <v>3.1</v>
+      </c>
+      <c r="G6">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D7">
+        <f>$C$7*((I7*($D$6-2.044)))/(1+(I7*($D$6-2.044)))</f>
+        <v>0.33279462535531795</v>
+      </c>
+      <c r="E7">
+        <f>C7*((I7*($E$6-2.044)))/(1+(I7*($E$6-2.044)))</f>
+        <v>0.29109858003989464</v>
+      </c>
+      <c r="F7">
+        <f>C7*((I7*($F$6-2.044)))/(1+(I7*($F$6-2.044)))</f>
+        <v>0.24039736293027167</v>
+      </c>
+      <c r="G7">
+        <f>C7*((I7*($G$6-2.044)))/(1+(I7*($G$6-2.044)))</f>
+        <v>0.19897861826544505</v>
+      </c>
+      <c r="I7">
+        <v>1.827</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D9" si="0">$C$7*((I8*($D$6-2.044)))/(1+(I8*($D$6-2.044)))</f>
+        <v>0.3290844183446951</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E15" si="1">C8*((I8*($E$6-2.044)))/(1+(I8*($E$6-2.044)))</f>
+        <v>0.28375745650741646</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F15" si="2">C8*((I8*($F$6-2.044)))/(1+(I8*($F$6-2.044)))</f>
+        <v>0.23034942745838746</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G15" si="3">C8*((I8*($G$6-2.044)))/(1+(I8*($G$6-2.044)))</f>
+        <v>0.18804917778467267</v>
+      </c>
+      <c r="I8">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.33861470706108032</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.30305121687776776</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.257522637971487</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.21832317445621077</v>
+      </c>
+      <c r="I9">
+        <v>2.2690000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="D10">
+        <f>$C$10/(((I10*($D$6-2.044)))/(1+(I10*($D$6-2.044))))</f>
+        <v>7.0083764048466765E-2</v>
+      </c>
+      <c r="E10">
+        <f>C10/(((I10*($E$6-2.044)))/(1+(I10*($E$6-2.044))))</f>
+        <v>8.0122342049224526E-2</v>
+      </c>
+      <c r="F10">
+        <f>C10/(((I10*($F$6-2.044)))/(1+(I10*($F$6-2.044))))</f>
+        <v>9.7020615017166745E-2</v>
+      </c>
+      <c r="G10">
+        <f>C10/(((I10*($G$6-2.044)))/(1+(I10*($G$6-2.044))))</f>
+        <v>0.11721611197885375</v>
+      </c>
+      <c r="I10">
+        <v>1.827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D12" si="4">$C$10/(((I11*($D$6-2.044)))/(1+(I11*($D$6-2.044))))</f>
+        <v>7.0873911676881965E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E12" si="5">C11/(((I11*($E$6-2.044)))/(1+(I11*($E$6-2.044))))</f>
+        <v>8.2195196866625436E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F12" si="6">C11/(((I11*($F$6-2.044)))/(1+(I11*($F$6-2.044))))</f>
+        <v>0.10125269360269359</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G12" si="7">C11/(((I11*($G$6-2.044)))/(1+(I11*($G$6-2.044))))</f>
+        <v>0.12402872628726286</v>
+      </c>
+      <c r="I11">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>6.3899999999999998E-2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>6.8879170082216307E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="5"/>
+        <v>7.6962238397502519E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="6"/>
+        <v>9.0568736728234289E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="7"/>
+        <v>0.10683016156252351</v>
+      </c>
+      <c r="I12">
+        <v>2.2690000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <f>$C$13/(((I13*($D$6-2.044)))/(1+(I13*($D$6-2.044))))</f>
+        <v>3.2245112097416637E-2</v>
+      </c>
+      <c r="E13">
+        <f>C13/(((I13*($E$6-2.044)))/(1+(I13*($E$6-2.044))))</f>
+        <v>3.686380056724884E-2</v>
+      </c>
+      <c r="F13">
+        <f>C13/(((I13*($F$6-2.044)))/(1+(I13*($F$6-2.044))))</f>
+        <v>4.4638592824799719E-2</v>
+      </c>
+      <c r="G13">
+        <f>C13/(((I13*($G$6-2.044)))/(1+(I13*($G$6-2.044))))</f>
+        <v>5.3930417717970268E-2</v>
+      </c>
+      <c r="I13">
+        <v>1.827</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D15" si="8">$C$13/(((I14*($D$6-2.044)))/(1+(I14*($D$6-2.044))))</f>
+        <v>3.2608654198753209E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E15" si="9">C14/(((I14*($E$6-2.044)))/(1+(I14*($E$6-2.044))))</f>
+        <v>3.7817508417508416E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F15" si="10">C14/(((I14*($F$6-2.044)))/(1+(I14*($F$6-2.044))))</f>
+        <v>4.658574635241302E-2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G15" si="11">C14/(((I14*($G$6-2.044)))/(1+(I14*($G$6-2.044))))</f>
+        <v>5.7064859981933141E-2</v>
+      </c>
+      <c r="I14">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="8"/>
+        <v>3.1690885765526748E-2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="9"/>
+        <v>3.5409856164109139E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="10"/>
+        <v>4.167012300172282E-2</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="11"/>
+        <v>4.9151905319846492E-2</v>
+      </c>
+      <c r="I15">
+        <v>2.2690000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>